<commit_message>
Feito exercicios 3 e 4
</commit_message>
<xml_diff>
--- a/exercicios_algoritmos.xlsx
+++ b/exercicios_algoritmos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programação\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programação\Python\Exercícios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46E29843-485D-4F83-8106-6604F7F7FF6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A07077-4777-469D-ABA9-882A03D0D8C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -489,7 +489,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,7 +523,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -531,7 +531,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Feito exercícios 7, 8, 9 e 10
</commit_message>
<xml_diff>
--- a/exercicios_algoritmos.xlsx
+++ b/exercicios_algoritmos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programação\Python\Exercícios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A07077-4777-469D-ABA9-882A03D0D8C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3DB55D-9C6C-405A-BC67-EAD138FC3C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,7 +101,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +111,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -153,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -165,6 +173,7 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +548,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -547,15 +556,15 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -563,7 +572,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -571,7 +580,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -579,7 +588,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -696,5 +705,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Feito do 11 ao 14
</commit_message>
<xml_diff>
--- a/exercicios_algoritmos.xlsx
+++ b/exercicios_algoritmos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programação\Python\Exercícios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3DB55D-9C6C-405A-BC67-EAD138FC3C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9719FB26-39EE-42FF-B931-9D53DE39A5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,7 +596,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -604,7 +604,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -620,7 +620,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Feito exercícios do 15 ao 20
</commit_message>
<xml_diff>
--- a/exercicios_algoritmos.xlsx
+++ b/exercicios_algoritmos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programação\Python\Exercícios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\teste\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9719FB26-39EE-42FF-B931-9D53DE39A5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBA3EB9-98DA-41AD-AAA1-D70E35AB6D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,9 +76,6 @@
     <t>Faça um algoritmo que leia uma temperatura em Fahrenheit e calcule a temperatura correspondente em grau Celsius. Imprima na tela as duas temperaturas.</t>
   </si>
   <si>
-    <t>Francisco tem 1,50m e cresce 2 centímetros por ano, enquanto Sara tem 1,10m e cresce 3 centímetros por ano. Faça um algoritmo que calcule e imprima na tela em quantos anos serão necessários para que Francisco seja maior que Sara.</t>
-  </si>
-  <si>
     <t>Faça um algoritmo que imprima na tela a tabuada de 1 até 10.</t>
   </si>
   <si>
@@ -95,6 +92,9 @@
   </si>
   <si>
     <t>Faça um algoritmo que calcule a quantidade de litros de combustível gastos em uma viagem, sabendo que o carro faz 12km com um litro.</t>
+  </si>
+  <si>
+    <t>Francisco tem 1,50m e cresce 2 centímetros por ano, enquanto Sara tem 1,10m e cresce 3 centímetros por ano. Faça um algoritmo que calcule e imprima na tela em quantos anos serão necessários para que Sara seja maior que Francisco.</t>
   </si>
 </sst>
 </file>
@@ -161,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -174,6 +174,7 @@
       </extLst>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +561,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="b">
@@ -592,7 +593,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="b">
@@ -624,11 +625,11 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -636,52 +637,52 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B20" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B21" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B22" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B22" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>22</v>
       </c>
       <c r="B23" s="2" t="b">
         <v>0</v>
@@ -689,7 +690,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="2" t="b">
         <v>0</v>
@@ -697,7 +698,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Feito Exercicio 23 e 24|| Finalizado Lista
</commit_message>
<xml_diff>
--- a/exercicios_algoritmos.xlsx
+++ b/exercicios_algoritmos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programação\Python\Exercicios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programação\Python\Exercícios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C7E3F1-5D82-4E8A-A014-5AA5976C3C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3A625E-238F-44EB-86C7-DC1E783F7206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +111,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -153,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -165,7 +173,15 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,7 +688,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="2" t="b">
@@ -680,19 +696,19 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="2" t="b">
-        <v>0</v>
+      <c r="B25" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>